<commit_message>
test ddqn case2 new complex
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/tested_state_original_design_case1.xlsx
+++ b/dynamics/src/dynamics/xlsx/tested_state_original_design_case1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,17 +424,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>0-A-0</t>
+          <t>0-C-0</t>
         </is>
       </c>
       <c r="B1" t="n">
         <v>0</v>
       </c>
       <c r="C1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D1" t="n">
-        <v>0.02178829349905755</v>
+        <v>0.01112081887113899</v>
       </c>
       <c r="E1" t="n">
         <v>26.036</v>
@@ -452,17 +452,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0-B-0</t>
+          <t>1-C-0</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0.6</v>
       </c>
       <c r="D2" t="n">
-        <v>0.006811749575498305</v>
+        <v>0.01112081887113899</v>
       </c>
       <c r="E2" t="n">
         <v>26.036</v>
@@ -480,17 +480,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1-A-0</t>
+          <t>2-C-0</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02178829349905755</v>
+        <v>0.01112081887113899</v>
       </c>
       <c r="E3" t="n">
         <v>26.036</v>
@@ -508,7 +508,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1-B-0</t>
+          <t>3-C-0</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -518,7 +518,7 @@
         <v>0.6</v>
       </c>
       <c r="D4" t="n">
-        <v>0.006811749575498305</v>
+        <v>0.01112081887113899</v>
       </c>
       <c r="E4" t="n">
         <v>26.036</v>
@@ -536,17 +536,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2-A-0</t>
+          <t>4-C-0</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02178829349905755</v>
+        <v>0.01112081887113899</v>
       </c>
       <c r="E5" t="n">
         <v>26.036</v>
@@ -564,17 +564,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2-B-0</t>
+          <t>5-C-0</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>0.6</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006811749575498305</v>
+        <v>0.01112081887113899</v>
       </c>
       <c r="E6" t="n">
         <v>26.036</v>
@@ -586,174 +586,6 @@
         <v>25.3</v>
       </c>
       <c r="H6" t="n">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>3-A-0</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.02178829349905755</v>
-      </c>
-      <c r="E7" t="n">
-        <v>26.036</v>
-      </c>
-      <c r="F7" t="n">
-        <v>23.964</v>
-      </c>
-      <c r="G7" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="H7" t="n">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>3-B-0</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.006811749575498305</v>
-      </c>
-      <c r="E8" t="n">
-        <v>26.036</v>
-      </c>
-      <c r="F8" t="n">
-        <v>23.964</v>
-      </c>
-      <c r="G8" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="H8" t="n">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>4-A-0</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.02178829349905755</v>
-      </c>
-      <c r="E9" t="n">
-        <v>26.036</v>
-      </c>
-      <c r="F9" t="n">
-        <v>23.964</v>
-      </c>
-      <c r="G9" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="H9" t="n">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>4-B-0</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.006811749575498305</v>
-      </c>
-      <c r="E10" t="n">
-        <v>26.036</v>
-      </c>
-      <c r="F10" t="n">
-        <v>23.964</v>
-      </c>
-      <c r="G10" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="H10" t="n">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>5-A-0</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.02178829349905755</v>
-      </c>
-      <c r="E11" t="n">
-        <v>26.036</v>
-      </c>
-      <c r="F11" t="n">
-        <v>23.964</v>
-      </c>
-      <c r="G11" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="H11" t="n">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>5-B-0</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.006811749575498305</v>
-      </c>
-      <c r="E12" t="n">
-        <v>26.036</v>
-      </c>
-      <c r="F12" t="n">
-        <v>23.964</v>
-      </c>
-      <c r="G12" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="H12" t="n">
         <v>25.3</v>
       </c>
     </row>

</xml_diff>